<commit_message>
Ajustes finais no rmd
</commit_message>
<xml_diff>
--- a/BigData/projeto_final_dicionário.xlsx
+++ b/BigData/projeto_final_dicionário.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4417308-4A85-4812-8FB2-C755D0662ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3395BF-0C9B-4219-93DD-3F8740A91480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t>Atraso (DEP_DELAY + ARR_DELAY) &gt; 0</t>
-  </si>
-  <si>
-    <t>MONTH</t>
   </si>
   <si>
     <t>Mês FL_DATE</t>
@@ -316,7 +313,10 @@
                    .otherwise("near"</t>
   </si>
   <si>
-    <t>Filtrar  e remover voos cancelados</t>
+    <t>FL_MONTH</t>
+  </si>
+  <si>
+    <t>Filtrar, remover voos cancelados e Excluir</t>
   </si>
 </sst>
 </file>
@@ -430,10 +430,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1033,7 @@
       <c r="D20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="16" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1050,7 +1050,8 @@
       <c r="D21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1098,9 +1099,6 @@
       <c r="D24" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E24" t="s">
-        <v>83</v>
-      </c>
       <c r="F24" t="s">
         <v>85</v>
       </c>
@@ -1152,7 +1150,7 @@
       <c r="E27" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1172,7 +1170,7 @@
       <c r="E28" t="s">
         <v>84</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1192,7 +1190,7 @@
       <c r="E29" t="s">
         <v>84</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1212,7 +1210,7 @@
       <c r="E30" t="s">
         <v>84</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1232,7 +1230,7 @@
       <c r="E31" t="s">
         <v>84</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1246,34 +1244,34 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
         <v>89</v>
-      </c>
-      <c r="B34" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
         <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
         <v>93</v>
-      </c>
-      <c r="B36" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>